<commit_message>
initial update - need wait for submission window to open
</commit_message>
<xml_diff>
--- a/Multi Files/emailTemplate.xlsx
+++ b/Multi Files/emailTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Documents\UiPath\Multi Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C363AB99-4F2C-4EE6-87AC-0DD36FAD99BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973BB874-E4BD-4005-8CE9-A19C8E8E828C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12972" yWindow="4116" windowWidth="12396" windowHeight="9000" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
+    <workbookView xWindow="132" yWindow="6864" windowWidth="12396" windowHeight="9000" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Alpha</t>
   </si>
@@ -71,6 +71,18 @@
   <si>
     <t>This email is sent by an UiPath Orchestrator bot.
 Regards</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Delt</t>
+  </si>
+  <si>
+    <t>Echo</t>
   </si>
 </sst>
 </file>
@@ -115,9 +127,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -447,13 +458,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E9B932-F46E-4292-B019-FC95463D2DDD}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
@@ -482,100 +493,122 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="F3" s="2"/>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="1"/>
-      <c r="F4" s="2"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
-      <c r="F5" s="2"/>
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F6" s="2"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F7" s="2"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F9" s="2"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F10" s="2"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F11" s="2"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F12" s="2"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F13" s="2"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F14" s="2"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F15" s="2"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="2"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F18" s="2"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="2"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F20" s="2"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F21" s="2"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F22" s="2"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F23" s="2"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F24" s="2"/>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FBB74F0F-5572-4568-B26E-53B5E8BC5E74}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{F1C875B4-CDC9-493B-815A-088A7212AAB9}"/>
+    <hyperlink ref="B3:B6" r:id="rId3" display="xiaodiz572@hotmail.com" xr:uid="{30A6DC1A-0E1E-4E98-A0AE-5A2467CF2626}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
eemail job application screenshots to recipents, classify into folders, generate excel report
</commit_message>
<xml_diff>
--- a/Multi Files/emailTemplate.xlsx
+++ b/Multi Files/emailTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Documents\UiPath\Multi Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973BB874-E4BD-4005-8CE9-A19C8E8E828C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ACDD72-81A1-4E17-BC16-BB774C71287A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="6864" windowWidth="12396" windowHeight="9000" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
+    <workbookView xWindow="3096" yWindow="372" windowWidth="23040" windowHeight="15228" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t>Alpha</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>RoboKiat</t>
   </si>
@@ -48,13 +45,7 @@
     <t>zephytk@gmail.com</t>
   </si>
   <si>
-    <t>Job Application Screenshots- Tse Kiat</t>
-  </si>
-  <si>
     <t>Recipent Name</t>
-  </si>
-  <si>
-    <t>Recipent email</t>
   </si>
   <si>
     <t>Subject  Header</t>
@@ -73,16 +64,16 @@
 Regards</t>
   </si>
   <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Charlie</t>
-  </si>
-  <si>
-    <t>Delt</t>
-  </si>
-  <si>
-    <t>Echo</t>
+    <t>Tse Kiat - Job Application Screenshots</t>
+  </si>
+  <si>
+    <t>Recipent Email</t>
+  </si>
+  <si>
+    <t>Ibnur</t>
+  </si>
+  <si>
+    <t>Tse Kiat</t>
   </si>
 </sst>
 </file>
@@ -466,50 +457,50 @@
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.08203125" customWidth="1"/>
+    <col min="6" max="6" width="38.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -517,35 +508,20 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
email body included date reference for job application
</commit_message>
<xml_diff>
--- a/Multi Files/emailTemplate.xlsx
+++ b/Multi Files/emailTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaod\Documents\UiPath\Multi Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ACDD72-81A1-4E17-BC16-BB774C71287A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367E0E7C-BB71-4186-9804-B184C97401AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="372" windowWidth="23040" windowHeight="15228" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12660" xr2:uid="{25D545AF-F4DF-443A-9AF0-D6B814F61477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>RoboKiat</t>
   </si>
@@ -60,20 +60,25 @@
     <t>Body</t>
   </si>
   <si>
-    <t>This email is sent by an UiPath Orchestrator bot.
+    <t>Tse Kiat - Job Application Screenshots</t>
+  </si>
+  <si>
+    <t>Recipent Email</t>
+  </si>
+  <si>
+    <t>Ibnur</t>
+  </si>
+  <si>
+    <t>Tse Kiat</t>
+  </si>
+  <si>
+    <t>Job application(s) submitted from :
+{0}
+This email is sent by an UiPath Orchestrator bot.
 Regards</t>
   </si>
   <si>
-    <t>Tse Kiat - Job Application Screenshots</t>
-  </si>
-  <si>
-    <t>Recipent Email</t>
-  </si>
-  <si>
-    <t>Ibnur</t>
-  </si>
-  <si>
-    <t>Tse Kiat</t>
+    <t xml:space="preserve"> ibnur@raceacademy.com.sg </t>
   </si>
 </sst>
 </file>
@@ -450,7 +455,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -468,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -485,13 +490,13 @@
     </row>
     <row r="2" spans="1:6" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -500,12 +505,12 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -580,11 +585,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FBB74F0F-5572-4568-B26E-53B5E8BC5E74}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{F1C875B4-CDC9-493B-815A-088A7212AAB9}"/>
-    <hyperlink ref="B3:B6" r:id="rId3" display="xiaodiz572@hotmail.com" xr:uid="{30A6DC1A-0E1E-4E98-A0AE-5A2467CF2626}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F1C875B4-CDC9-493B-815A-088A7212AAB9}"/>
+    <hyperlink ref="B3:B6" r:id="rId2" display="xiaodiz572@hotmail.com" xr:uid="{30A6DC1A-0E1E-4E98-A0AE-5A2467CF2626}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>